<commit_message>
Actualizacion de gato y quiniela
</commit_message>
<xml_diff>
--- a/QuinielaM.xlsx
+++ b/QuinielaM.xlsx
@@ -1,52 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Participantes" sheetId="1" r:id="rId1"/>
+    <sheet name="Participantes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,13 +42,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,271 +440,404 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Qatar</v>
-      </c>
-      <c r="B1" t="str">
-        <v>0</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>Ecuador</v>
-      </c>
-      <c r="B2" t="str">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>Senegal</v>
-      </c>
-      <c r="B3" t="str">
-        <v>0</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Senegal</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
-        <v>Paises Bajos</v>
-      </c>
-      <c r="B4" t="str">
-        <v>0</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Paises Bajos</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
-        <v>Inglaterra</v>
-      </c>
-      <c r="B5" t="str">
-        <v>0</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Inglaterra</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
-        <v>Iran</v>
-      </c>
-      <c r="B6" t="str">
-        <v>0</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Iran</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
-        <v>Estados Unidos</v>
-      </c>
-      <c r="B7" t="str">
-        <v>0</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Estados Unidos</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
-        <v>Gales</v>
-      </c>
-      <c r="B8" t="str">
-        <v>0</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gales</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
-        <v>Argentina</v>
-      </c>
-      <c r="B9" t="str">
-        <v>0</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
-        <v>Arabia Saudita</v>
-      </c>
-      <c r="B10" t="str">
-        <v>0</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Arabia Saudita</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
-        <v>Mexico</v>
-      </c>
-      <c r="B11" t="str">
-        <v>0</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
-        <v>Polonia</v>
-      </c>
-      <c r="B12" t="str">
-        <v>0</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Polonia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
-        <v>Francia</v>
-      </c>
-      <c r="B13" t="str">
-        <v>0</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Francia</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
-        <v>Australia</v>
-      </c>
-      <c r="B14" t="str">
-        <v>0</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
-        <v>Dinamarca</v>
-      </c>
-      <c r="B15" t="str">
-        <v>0</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Dinamarca</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
-        <v>Tunez</v>
-      </c>
-      <c r="B16" t="str">
-        <v>0</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Tunez</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
-        <v>España</v>
-      </c>
-      <c r="B17" t="str">
-        <v>0</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
-        <v>Costa Rica</v>
-      </c>
-      <c r="B18" t="str">
-        <v>0</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
-        <v>Alemania</v>
-      </c>
-      <c r="B19" t="str">
-        <v>0</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Alemania</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="str">
-        <v>Japon</v>
-      </c>
-      <c r="B20" t="str">
-        <v>0</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Japon</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="str">
-        <v>Belgica</v>
-      </c>
-      <c r="B21" t="str">
-        <v>0</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Belgica</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="str">
-        <v>Canda</v>
-      </c>
-      <c r="B22" t="str">
-        <v>0</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Canda</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="str">
-        <v>Marruecos</v>
-      </c>
-      <c r="B23" t="str">
-        <v>0</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Marruecos</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="str">
-        <v>Croacia</v>
-      </c>
-      <c r="B24" t="str">
-        <v>0</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Croacia</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="str">
-        <v>Brasil</v>
-      </c>
-      <c r="B25" t="str">
-        <v>0</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="str">
-        <v>Serbia</v>
-      </c>
-      <c r="B26" t="str">
-        <v>0</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Serbia</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="str">
-        <v>Suiza</v>
-      </c>
-      <c r="B27" t="str">
-        <v>0</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Suiza</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="str">
-        <v>Cameron</v>
-      </c>
-      <c r="B28" t="str">
-        <v>0</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Cameron</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="str">
-        <v>Portugal</v>
-      </c>
-      <c r="B29" t="str">
-        <v>0</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="str">
-        <v>Ghana</v>
-      </c>
-      <c r="B30" t="str">
-        <v>0</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Ghana</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="str">
-        <v>Uruguay</v>
-      </c>
-      <c r="B31" t="str">
-        <v>0</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="str">
-        <v>Corea del Sur</v>
-      </c>
-      <c r="B32" t="str">
-        <v>0</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Corea del Sur</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B32"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustes para comparacion de grupo
</commit_message>
<xml_diff>
--- a/QuinielaM.xlsx
+++ b/QuinielaM.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>

</xml_diff>